<commit_message>
fix[format]: fix format bugs in fp32 and bf16
</commit_message>
<xml_diff>
--- a/bf16_add.xlsx
+++ b/bf16_add.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\InfiScale\tpu_module_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BED2E6A-42DE-4284-A834-0A84E586D157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A69978-D7D5-4689-ADBE-75EE9346F1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27975" yWindow="8265" windowWidth="19200" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x4000</t>
+    <t>0x0040</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -341,12 +341,15 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -369,9 +372,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,7 +666,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:F29"/>
+      <selection activeCell="D10" sqref="D10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -675,136 +675,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -820,338 +820,265 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="11"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="11"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="11"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="11"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="11"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="11"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="11"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="11"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="11"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="11"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="11"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="11"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="11"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="11"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="11"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A17:B17"/>
@@ -1166,6 +1093,79 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>